<commit_message>
Outputting tables to word document
</commit_message>
<xml_diff>
--- a/Lab3/data.xlsx
+++ b/Lab3/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\ENGO634\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F87B69-B711-4EB7-825F-BCBB4B7BFC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29621393-D7D3-4733-95A7-74EFA0ADBAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="4725" windowWidth="17535" windowHeight="11265" xr2:uid="{A516DE37-B4A4-4C43-A01A-9ACF9A515E2C}"/>
+    <workbookView xWindow="-18705" yWindow="4830" windowWidth="17535" windowHeight="11265" xr2:uid="{A516DE37-B4A4-4C43-A01A-9ACF9A515E2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFEF962D-3CE0-4463-B8D5-AED0801EEE52}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E23" sqref="B18:E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>